<commit_message>
Sequence Diagram 3 e 4
</commit_message>
<xml_diff>
--- a/quarto use case.xlsx
+++ b/quarto use case.xlsx
@@ -36,9 +36,6 @@
     <t>Exceptions</t>
   </si>
   <si>
-    <t>Taxi Driver, user1, user2, user 3</t>
-  </si>
-  <si>
     <t>User1, user 2 and user 3 have requests a taxi in the same zone, have the sharing option active and must to go in the same direction</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Shared taxi request</t>
+  </si>
+  <si>
+    <t>Taxi Driver, user1, user2, user 3, taximeter</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -439,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -455,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -463,57 +463,57 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -521,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -529,22 +529,22 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>